<commit_message>
Working on the letter Sternberg task
The aim is to get the LetStern task working. Then fork it and make the
partial trial implementation of it.
</commit_message>
<xml_diff>
--- a/LetterSternberg/LetterSternbergConditions.xlsx
+++ b/LetterSternberg/LetterSternbergConditions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="11100" yWindow="4380" windowWidth="16620" windowHeight="8300" tabRatio="500"/>
@@ -21,31 +21,31 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
+    <t>ITI</t>
+  </si>
+  <si>
+    <t>A B C</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>D F G H B N M</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>StimLetters</t>
+  </si>
+  <si>
     <t>ProbeLetter</t>
-  </si>
-  <si>
-    <t>ITI</t>
-  </si>
-  <si>
-    <t>A B C</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>D F G H B N M</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>StimLetters</t>
   </si>
 </sst>
 </file>
@@ -417,28 +417,31 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -446,10 +449,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>7</v>
@@ -457,10 +460,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
       </c>
       <c r="C4">
         <v>1</v>

</xml_diff>

<commit_message>
working on let stern
</commit_message>
<xml_diff>
--- a/LetterSternberg/LetterSternbergConditions.xlsx
+++ b/LetterSternberg/LetterSternbergConditions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>A B C</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>ProbeLetter</t>
+  </si>
+  <si>
+    <t>ITI</t>
   </si>
 </sst>
 </file>
@@ -411,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -422,36 +425,48 @@
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>